<commit_message>
Fix per semantici per accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#FRAMESRLXX/FRAMESRL/GOMED-PEDIATOTEM/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111#FRAMESRLXX/FRAMESRL/GOMED-PEDIATOTEM/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39339\Desktop\FSE\S1#111#FRAMESRLXX\FRAMESRL\GOMED-PEDIATOTEM\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1987D45-98D8-4094-A665-4939FC51396B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E97C6AC-6559-4048-99CE-BD975F56FC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1779,34 +1779,34 @@
     <t>Frame S.r.l.</t>
   </si>
   <si>
-    <t>2025-06-19T13:30:35.94120470</t>
-  </si>
-  <si>
-    <t>2025-06-19T13:30:35.308092200</t>
-  </si>
-  <si>
-    <t>d9e92cd6f54e302c96bb1122b68a2f8d</t>
-  </si>
-  <si>
-    <t>4427644f730a89f779103946d9231879</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120.4.4.15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225.d30175944e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120.4.4.15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225.da53ade124^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-06-20T10:16:02.420388500</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120.4.4.15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225.977b85801e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>be37a1f39ecf5b96c23ca273cb599179</t>
-  </si>
-  <si>
     <t>subject_application_id:GOMED-PEDIATOTEM</t>
+  </si>
+  <si>
+    <t>82f1f023ba5dab3da9f752a0d9bb740c</t>
+  </si>
+  <si>
+    <t>2025-06-26T17:12:22.827649400</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120.4.4.15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225.12da91777c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-06-26T17:12:23.553906200</t>
+  </si>
+  <si>
+    <t>3ff4b041f204ed8a115f7cdcd5f24c76</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120.4.4.15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225.401649b407^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120.4.4.15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225.f405dc5d99^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6045d6dfd329727f92577dfe7f6db5a1</t>
+  </si>
+  <si>
+    <t>2025-06-26T17:12:24.181275800</t>
   </si>
 </sst>
 </file>
@@ -3876,10 +3876,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I132" sqref="I132"/>
+      <selection pane="bottomRight" activeCell="H165" sqref="H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="B3" s="51"/>
       <c r="C3" s="56" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="D3" s="48"/>
       <c r="F3" s="6"/>
@@ -8749,16 +8749,16 @@
         <v>344</v>
       </c>
       <c r="F132" s="37">
-        <v>45828</v>
+        <v>45834</v>
       </c>
       <c r="G132" s="37" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H132" s="37" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="I132" s="42" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="J132" s="38" t="s">
         <v>64</v>
@@ -10033,16 +10033,16 @@
         <v>243</v>
       </c>
       <c r="F164" s="37">
-        <v>45827</v>
+        <v>45834</v>
       </c>
       <c r="G164" s="37" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="H164" s="37" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="I164" s="42" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="J164" s="38" t="s">
         <v>64</v>
@@ -10082,16 +10082,16 @@
         <v>244</v>
       </c>
       <c r="F165" s="37">
-        <v>45827</v>
+        <v>45834</v>
       </c>
       <c r="G165" s="37" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="H165" s="37" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="I165" s="42" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="J165" s="38" t="s">
         <v>64</v>
@@ -17424,6 +17424,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17681,28 +17702,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17721,31 +17746,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>